<commit_message>
Edited the to do list, put google maps into the Vietnam page
</commit_message>
<xml_diff>
--- a/team-kaye-to-do-list.xlsx
+++ b/team-kaye-to-do-list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F8CA8-0E17-4A9F-AAF5-8AC699989AFC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F05DDB-5C42-48F6-B2A3-78CAC49122C7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>About Us</t>
   </si>
@@ -102,10 +102,13 @@
     <t>make it like switzerland page</t>
   </si>
   <si>
-    <t>Carousel JavaScript</t>
-  </si>
-  <si>
     <t xml:space="preserve">bootstrap </t>
+  </si>
+  <si>
+    <t>add in actual google maps api?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carousel JavaScript - https://getbootstrap.com/docs/3.3/javascript/#carousel </t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="F3:W21"/>
+  <dimension ref="F3:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="6:23" x14ac:dyDescent="0.35">
@@ -535,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.35">
@@ -557,6 +560,11 @@
       </c>
       <c r="H21" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Vietnam with footer
</commit_message>
<xml_diff>
--- a/team-kaye-to-do-list.xlsx
+++ b/team-kaye-to-do-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B792BB29-5931-444D-A668-0B5749DF928E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E7A55-6611-4023-B417-C431C5BA8214}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F3:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
edited Switzerland carousel and updated to do list
</commit_message>
<xml_diff>
--- a/team-kaye-to-do-list.xlsx
+++ b/team-kaye-to-do-list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kat\Documents\CFG\TeamKV2\team-kaye\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946C01E-2F56-4405-9D9A-CA8103E99B4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>About Us</t>
   </si>
@@ -57,9 +58,6 @@
     <t>Contact us form</t>
   </si>
   <si>
-    <t>Sort kaylee photo</t>
-  </si>
-  <si>
     <t>Destinations</t>
   </si>
   <si>
@@ -102,9 +100,6 @@
     <t xml:space="preserve">bootstrap </t>
   </si>
   <si>
-    <t>add in actual google maps api?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carousel JavaScript - https://getbootstrap.com/docs/3.3/javascript/#carousel </t>
   </si>
   <si>
@@ -121,12 +116,33 @@
   </si>
   <si>
     <t>Optional: drop down menu</t>
+  </si>
+  <si>
+    <t>Sort Kathryn photo</t>
+  </si>
+  <si>
+    <t>transfer jpeg to imgur</t>
+  </si>
+  <si>
+    <t>add in actual google maps api</t>
+  </si>
+  <si>
+    <t>add marker to google maps page</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>edit on destinations pages to look more suited</t>
+  </si>
+  <si>
+    <t>dropdown menu on destinations menu bit?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,12 +161,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,9 +187,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,16 +470,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:W25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="F3:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
@@ -476,17 +499,17 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="6:23" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -497,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:23" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
         <v>7</v>
       </c>
@@ -505,91 +528,112 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="6:23" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="6:23" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="6:23" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="6:23" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="6:23" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="6:23" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" t="s">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H24" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
+      <c r="H27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" t="s">
-        <v>29</v>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -599,18 +643,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bout us update reposiveness
</commit_message>
<xml_diff>
--- a/team-kaye-to-do-list.xlsx
+++ b/team-kaye-to-do-list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kat\Documents\CFG\TeamKV2\team-kaye\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946C01E-2F56-4405-9D9A-CA8103E99B4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,16 +469,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,18 +508,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:23" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>7</v>
       </c>
@@ -528,7 +527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>0</v>
       </c>
@@ -539,20 +538,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="6:23" x14ac:dyDescent="0.35">
-      <c r="H10" t="s">
+    <row r="10" spans="6:23" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="6:23" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>10</v>
       </c>
@@ -563,12 +562,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:23" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="6:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>16</v>
       </c>
@@ -579,7 +578,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H17" s="2" t="s">
         <v>18</v>
       </c>
@@ -587,17 +586,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>21</v>
       </c>
@@ -605,17 +604,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H23" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>26</v>
       </c>
@@ -623,7 +622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>34</v>
       </c>
@@ -631,28 +630,28 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
a few minor updates to the Vietnam page, first attempts at a drop-down menu for the destinations in the navigation bar
</commit_message>
<xml_diff>
--- a/team-kaye-to-do-list.xlsx
+++ b/team-kaye-to-do-list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kat\Documents\CFG\TeamKV2\team-kaye\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn\Documents\University\Third Year\Code First\Competition Page\team-kaye-master\team-kaye\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8019EC55-826A-4302-855C-9088354F7F0A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,16 +473,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F3:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
@@ -511,7 +512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -522,7 +523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:23" x14ac:dyDescent="0.35">
       <c r="H6" t="s">
         <v>7</v>
       </c>
@@ -530,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>0</v>
       </c>
@@ -541,7 +542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:23" x14ac:dyDescent="0.35">
       <c r="H10" s="2" t="s">
         <v>30</v>
       </c>
@@ -549,28 +550,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:23" x14ac:dyDescent="0.35">
       <c r="H11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:23" x14ac:dyDescent="0.35">
       <c r="H14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="6:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:23" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>16</v>
       </c>
@@ -581,7 +582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H17" s="2" t="s">
         <v>18</v>
       </c>
@@ -589,17 +590,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F22" t="s">
         <v>21</v>
       </c>
@@ -607,38 +608,38 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H23" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F29" t="s">
         <v>34</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:11" x14ac:dyDescent="0.35">
       <c r="H30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F32" t="s">
         <v>37</v>
       </c>
@@ -650,16 +651,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>28</v>
       </c>

</xml_diff>